<commit_message>
add note about role
</commit_message>
<xml_diff>
--- a/Document/Design/SRS + User Requirement/HaiTCT/Issue.xlsx
+++ b/Document/Design/SRS + User Requirement/HaiTCT/Issue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>No</t>
   </si>
@@ -42,18 +42,12 @@
     <t>Role in Project</t>
   </si>
   <si>
-    <t>Xai bang Assigment role la PROJECT_POSITION_CODE</t>
-  </si>
-  <si>
     <t>Project field</t>
   </si>
   <si>
     <t>Project Type, Bussiness Domain Project Status</t>
   </si>
   <si>
-    <t>1 la PM, 2 la DEVELOPER,,, TYPE moi dung'</t>
-  </si>
-  <si>
     <t>Xai table Bussiness Domain General_Reference</t>
   </si>
   <si>
@@ -139,6 +133,29 @@
   </si>
   <si>
     <t>baseline note for note.</t>
+  </si>
+  <si>
+    <t>risk table</t>
+  </si>
+  <si>
+    <t>sudung table risk</t>
+  </si>
+  <si>
+    <t>issue table</t>
+  </si>
+  <si>
+    <t>su dung table issue</t>
+  </si>
+  <si>
+    <t>workUnitID will be projectID</t>
+  </si>
+  <si>
+    <t>Xai bang Assigment role la Type</t>
+  </si>
+  <si>
+    <t>0: ProjectOwer + PM, 1 : pM, 2: dev, 3: test, 4 QA, 5 cus, 6: project Owner
+Project Owner chi co' quyen read only va change PM,
+User tao project se~ mang role la 0;</t>
   </si>
 </sst>
 </file>
@@ -181,10 +198,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -536,10 +556,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -547,13 +567,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -561,37 +581,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -599,21 +619,21 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,13 +641,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,13 +655,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,13 +669,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,10 +683,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,13 +694,38 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C16" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>